<commit_message>
Delete file saver, not used modified name of excel file
</commit_message>
<xml_diff>
--- a/Project/static/download_example/portfolio_construction_dataset.xlsx
+++ b/Project/static/download_example/portfolio_construction_dataset.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\Flask_London\Project\static\download_example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E6D38519-E13C-440E-9220-01C59A69E87A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D62A24-39B8-4944-BEF0-E5BFB6D09ACC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4C8E02F5-6FAD-495F-A07D-6CC1C3D723B6}"/>
   </bookViews>
@@ -397,7 +397,7 @@
   <dimension ref="A1:C2500"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="T32" sqref="T32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>